<commit_message>
Calculates Pearson correlation for each metric (#9)
* Fixed bug with ids in handlebars

* Adding correlation service

* Get data to correlate

* Pearson runs

* Calculates Pearson correlation for each metric

Co-authored-by: Gilles Fabre <gillesfabre34@gmail.com>
</commit_message>
<xml_diff>
--- a/src/core/mocks/siegmund-2012/dataset.xlsx
+++ b/src/core/mocks/siegmund-2012/dataset.xlsx
@@ -8,13 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utilisateur/Documents/projets/genese/metrics/src/core/mocks/siegmund-2012/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C59E0C1-A7B1-9F41-88D1-22F7350019A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C18B60-3DAF-6149-B297-F57AF1B45C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{6B2507F4-2ED4-784C-80A2-5B5CA1CAB9E0}"/>
+    <workbookView xWindow="41480" yWindow="2300" windowWidth="27640" windowHeight="16940" xr2:uid="{6B2507F4-2ED4-784C-80A2-5B5CA1CAB9E0}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.10" hidden="1">data!$E$4:$E$22</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">data!$B$4:$B$22</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">data!$E$3</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">data!$E$4:$E$22</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">data!$B$4:$B$22</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">data!$E$3</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">data!$E$4:$E$22</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">data!$B$4:$B$22</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">data!$E$3</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">data!$E$4:$E$22</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">data!$B$3</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">data!$B$4:$B$22</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">data!$E$3</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">data!$B$3</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">data!$B$4:$B$22</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">data!$E$3</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">data!$E$4:$E$22</definedName>
+  </definedNames>
   <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Siegmund 2012</t>
   </si>
@@ -109,6 +128,9 @@
   </si>
   <si>
     <t>snippet_id</t>
+  </si>
+  <si>
+    <t>LOC</t>
   </si>
 </sst>
 </file>
@@ -179,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -199,6 +221,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -214,6 +239,1050 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>test</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LOC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data!$B$4:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>68.014414634146334</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.26741463414632</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>154.64156097560979</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>211.48453658536584</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70.510951219512179</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>66.048609756097534</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>104.82602439024393</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>65.420853658536572</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42.585804878048783</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>65.473780487804873</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>59.81002439024391</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>37.425292682926823</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>48.394707317073163</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20.50239024390244</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>99.988414634146352</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>145.23982926829271</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80.621829268292686</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>89.939219512195123</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>54.500707317073157</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>data!$E$4:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-92CD-5241-A85C-4FD114D62F15}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1828947583"/>
+        <c:axId val="1518830015"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1828947583"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1518830015"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1518830015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1828947583"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>565150</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8699E071-EAAA-684F-96EF-17E07E227DB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -511,17 +1580,303 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/themeOverride1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线 Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E401E57-2C53-E249-A7ED-8E36F62BE131}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -529,13 +1884,13 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -548,8 +1903,11 @@
       <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E3" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -562,8 +1920,11 @@
       <c r="D4" s="4">
         <v>6.8</v>
       </c>
+      <c r="E4" s="7">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -576,8 +1937,11 @@
       <c r="D5" s="4">
         <v>18.100000000000001</v>
       </c>
+      <c r="E5" s="7">
+        <v>12</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -590,8 +1954,11 @@
       <c r="D6" s="4">
         <v>15.4</v>
       </c>
+      <c r="E6" s="7">
+        <v>11</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -604,8 +1971,11 @@
       <c r="D7" s="4">
         <v>14.3</v>
       </c>
+      <c r="E7" s="7">
+        <v>13</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -618,8 +1988,11 @@
       <c r="D8" s="4">
         <v>7.1</v>
       </c>
+      <c r="E8" s="7">
+        <v>6</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -632,8 +2005,11 @@
       <c r="D9" s="4">
         <v>9.5</v>
       </c>
+      <c r="E9" s="7">
+        <v>7</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -646,8 +2022,11 @@
       <c r="D10" s="4">
         <v>7.4</v>
       </c>
+      <c r="E10" s="7">
+        <v>8</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
@@ -660,8 +2039,11 @@
       <c r="D11" s="4">
         <v>8.9</v>
       </c>
+      <c r="E11" s="7">
+        <v>9</v>
+      </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
@@ -674,8 +2056,11 @@
       <c r="D12" s="4">
         <v>16.7</v>
       </c>
+      <c r="E12" s="7">
+        <v>10</v>
+      </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -688,8 +2073,11 @@
       <c r="D13" s="4">
         <v>7.4</v>
       </c>
+      <c r="E13" s="7">
+        <v>8</v>
+      </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
@@ -702,8 +2090,11 @@
       <c r="D14" s="4">
         <v>14</v>
       </c>
+      <c r="E14" s="7">
+        <v>10</v>
+      </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -716,8 +2107,11 @@
       <c r="D15" s="4">
         <v>6</v>
       </c>
+      <c r="E15" s="7">
+        <v>8</v>
+      </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -730,8 +2124,11 @@
       <c r="D16" s="4">
         <v>9.5</v>
       </c>
+      <c r="E16" s="7">
+        <v>6</v>
+      </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
@@ -744,8 +2141,11 @@
       <c r="D17" s="4">
         <v>5.6</v>
       </c>
+      <c r="E17" s="7">
+        <v>5</v>
+      </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
@@ -758,8 +2158,11 @@
       <c r="D18" s="4">
         <v>16.2</v>
       </c>
+      <c r="E18" s="7">
+        <v>14</v>
+      </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
@@ -772,8 +2175,11 @@
       <c r="D19" s="4">
         <v>21.3</v>
       </c>
+      <c r="E19" s="7">
+        <v>11</v>
+      </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
@@ -786,8 +2192,11 @@
       <c r="D20" s="4">
         <v>9.8000000000000007</v>
       </c>
+      <c r="E20" s="7">
+        <v>10</v>
+      </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
@@ -800,8 +2209,11 @@
       <c r="D21" s="4">
         <v>11.7</v>
       </c>
+      <c r="E21" s="7">
+        <v>9</v>
+      </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>22</v>
       </c>
@@ -814,8 +2226,11 @@
       <c r="D22" s="4">
         <v>9.6</v>
       </c>
+      <c r="E22" s="7">
+        <v>6</v>
+      </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="6" t="s">
         <v>23</v>
@@ -827,6 +2242,10 @@
       <c r="D23" s="6">
         <f>PEARSON($B4:$B22,D4:D22)</f>
         <v>0.55597715532437797</v>
+      </c>
+      <c r="E23" s="6">
+        <f>PEARSON($B4:$B22,E4:E22)</f>
+        <v>0.68585381728631001</v>
       </c>
     </row>
   </sheetData>
@@ -834,5 +2253,6 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>